<commit_message>
[ADD] migration 12.0 to 14.0
</commit_message>
<xml_diff>
--- a/car_workshop_base/static/description/brands_and_models.xlsx
+++ b/car_workshop_base/static/description/brands_and_models.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo" sheetId="1" state="visible" r:id="rId2"/>
@@ -2784,25 +2784,7 @@
     <t xml:space="preserve">Infiniti</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">fleet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.brand_infiniti</t>
-    </r>
+    <t xml:space="preserve">fleet.brand_infiniti</t>
   </si>
   <si>
     <t xml:space="preserve">Innocenti</t>
@@ -2868,7 +2850,7 @@
     <t xml:space="preserve">Land-rover</t>
   </si>
   <si>
-    <t xml:space="preserve">fleet.brand_land rover</t>
+    <t xml:space="preserve">fleet.brand_land_rover</t>
   </si>
   <si>
     <t xml:space="preserve">Ldv</t>
@@ -3082,7 +3064,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3118,12 +3100,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3168,7 +3144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3187,10 +3163,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3216,15 +3188,15 @@
   </sheetPr>
   <dimension ref="A1:C2009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="9.38"/>
   </cols>
   <sheetData>
@@ -8804,7 +8776,7 @@
       </c>
       <c r="C465" s="0" t="str">
         <f aca="false">VLOOKUP(B465,odoo,3,0)</f>
-        <v>fleet.brand_land rover</v>
+        <v>fleet.brand_land_rover</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8816,7 +8788,7 @@
       </c>
       <c r="C466" s="0" t="str">
         <f aca="false">VLOOKUP(B466,odoo,3,0)</f>
-        <v>fleet.brand_land rover</v>
+        <v>fleet.brand_land_rover</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8828,7 +8800,7 @@
       </c>
       <c r="C467" s="0" t="str">
         <f aca="false">VLOOKUP(B467,odoo,3,0)</f>
-        <v>fleet.brand_land rover</v>
+        <v>fleet.brand_land_rover</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8840,7 +8812,7 @@
       </c>
       <c r="C468" s="0" t="str">
         <f aca="false">VLOOKUP(B468,odoo,3,0)</f>
-        <v>fleet.brand_land rover</v>
+        <v>fleet.brand_land_rover</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8852,7 +8824,7 @@
       </c>
       <c r="C469" s="0" t="str">
         <f aca="false">VLOOKUP(B469,odoo,3,0)</f>
-        <v>fleet.brand_land rover</v>
+        <v>fleet.brand_land_rover</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8864,7 +8836,7 @@
       </c>
       <c r="C470" s="0" t="str">
         <f aca="false">VLOOKUP(B470,odoo,3,0)</f>
-        <v>fleet.brand_land rover</v>
+        <v>fleet.brand_land_rover</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8876,7 +8848,7 @@
       </c>
       <c r="C471" s="0" t="str">
         <f aca="false">VLOOKUP(B471,odoo,3,0)</f>
-        <v>fleet.brand_land rover</v>
+        <v>fleet.brand_land_rover</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19353,11 +19325,11 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
@@ -19405,7 +19377,7 @@
       <c r="B4" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>864</v>
       </c>
     </row>
@@ -19416,7 +19388,7 @@
       <c r="B5" s="2" t="s">
         <v>865</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>866</v>
       </c>
     </row>
@@ -19427,7 +19399,7 @@
       <c r="B6" s="2" t="s">
         <v>867</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>866</v>
       </c>
     </row>
@@ -19438,7 +19410,7 @@
       <c r="B7" s="2" t="s">
         <v>868</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>869</v>
       </c>
     </row>
@@ -19471,7 +19443,7 @@
       <c r="B10" s="2" t="s">
         <v>874</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>875</v>
       </c>
     </row>
@@ -19493,7 +19465,7 @@
       <c r="B12" s="2" t="s">
         <v>878</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>879</v>
       </c>
     </row>
@@ -19559,7 +19531,7 @@
       <c r="B18" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>890</v>
       </c>
     </row>
@@ -19570,7 +19542,7 @@
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>891</v>
       </c>
     </row>
@@ -19592,7 +19564,7 @@
       <c r="B21" s="2" t="s">
         <v>894</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>895</v>
       </c>
     </row>
@@ -19603,7 +19575,7 @@
       <c r="B22" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>897</v>
       </c>
     </row>
@@ -19614,7 +19586,7 @@
       <c r="B23" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>899</v>
       </c>
     </row>
@@ -19669,7 +19641,7 @@
       <c r="B28" s="2" t="s">
         <v>908</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>909</v>
       </c>
     </row>
@@ -19680,7 +19652,7 @@
       <c r="B29" s="2" t="s">
         <v>910</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>911</v>
       </c>
     </row>
@@ -19702,7 +19674,7 @@
       <c r="B31" s="2" t="s">
         <v>914</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>915</v>
       </c>
     </row>
@@ -19724,7 +19696,7 @@
       <c r="B33" s="2" t="s">
         <v>918</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>919</v>
       </c>
     </row>
@@ -19735,7 +19707,7 @@
       <c r="B34" s="2" t="s">
         <v>920</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>921</v>
       </c>
     </row>
@@ -19768,7 +19740,7 @@
       <c r="B37" s="2" t="s">
         <v>926</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>927</v>
       </c>
     </row>
@@ -19812,7 +19784,7 @@
       <c r="B41" s="2" t="s">
         <v>934</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>935</v>
       </c>
     </row>
@@ -19823,7 +19795,7 @@
       <c r="B42" s="2" t="s">
         <v>936</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="3" t="s">
         <v>937</v>
       </c>
     </row>
@@ -19856,7 +19828,7 @@
       <c r="B45" s="2" t="s">
         <v>942</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="3" t="s">
         <v>943</v>
       </c>
     </row>
@@ -19889,7 +19861,7 @@
       <c r="B48" s="2" t="s">
         <v>948</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>949</v>
       </c>
     </row>
@@ -20065,7 +20037,7 @@
       <c r="B64" s="2" t="s">
         <v>978</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>979</v>
       </c>
     </row>
@@ -20087,7 +20059,7 @@
       <c r="B66" s="2" t="s">
         <v>831</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="3" t="s">
         <v>982</v>
       </c>
     </row>
@@ -20131,7 +20103,7 @@
       <c r="B70" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="3" t="s">
         <v>989</v>
       </c>
     </row>
@@ -20164,7 +20136,7 @@
       <c r="B73" s="2" t="s">
         <v>994</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="3" t="s">
         <v>995</v>
       </c>
     </row>
@@ -20175,7 +20147,7 @@
       <c r="B74" s="2" t="s">
         <v>996</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="3" t="s">
         <v>997</v>
       </c>
     </row>
@@ -20197,7 +20169,7 @@
       <c r="B76" s="2" t="s">
         <v>1000</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="3" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -20208,7 +20180,7 @@
       <c r="B77" s="2" t="s">
         <v>1002</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="3" t="s">
         <v>1003</v>
       </c>
     </row>
@@ -20241,7 +20213,7 @@
       <c r="B80" s="2" t="s">
         <v>1008</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C80" s="3" t="s">
         <v>1009</v>
       </c>
     </row>

</xml_diff>